<commit_message>
Commit after take-home_ex04 v2
</commit_message>
<xml_diff>
--- a/Take-home_Ex/Take-home_Ex04/data/main.xlsx
+++ b/Take-home_Ex/Take-home_Ex04/data/main.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prach\Documents\VAA\PrachiRAshani\ISSS608-VAA\Take-home_Ex\Take-home_Ex04\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70DE8737-EA34-4A5A-B13F-94D65EFB7560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0548451E-A607-4C27-9DE9-8B14419B5815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{75DF03A9-EE48-4C33-9E41-358D67B76907}"/>
   </bookViews>
@@ -36,12 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="117">
   <si>
     <t>Country</t>
-  </si>
-  <si>
-    <t>Type</t>
   </si>
   <si>
     <t>Belgium</t>
@@ -389,120 +386,16 @@
     <t>Trade Balance</t>
   </si>
   <si>
-    <t>Nov 2022</t>
-  </si>
-  <si>
-    <t>Dec 2022</t>
-  </si>
-  <si>
-    <t>Oct 2022</t>
-  </si>
-  <si>
-    <t>Sep 2022</t>
-  </si>
-  <si>
-    <t>Aug 2022</t>
-  </si>
-  <si>
-    <t>Jul 2022</t>
-  </si>
-  <si>
-    <t>Jun 2022</t>
-  </si>
-  <si>
-    <t>May 2022</t>
-  </si>
-  <si>
-    <t>Apr 2022</t>
-  </si>
-  <si>
-    <t>Mar 2022</t>
-  </si>
-  <si>
-    <t>Feb 2022</t>
-  </si>
-  <si>
-    <t>Jan 2022</t>
-  </si>
-  <si>
-    <t>Dec 2021</t>
-  </si>
-  <si>
-    <t>Nov 2021</t>
-  </si>
-  <si>
-    <t>Oct 2021</t>
-  </si>
-  <si>
-    <t>Sep 2021</t>
-  </si>
-  <si>
-    <t>Aug 2021</t>
-  </si>
-  <si>
-    <t>Jul 2021</t>
-  </si>
-  <si>
-    <t>Jun 2021</t>
-  </si>
-  <si>
-    <t>May 2021</t>
-  </si>
-  <si>
-    <t>Apr 2021</t>
-  </si>
-  <si>
-    <t>Mar 2021</t>
-  </si>
-  <si>
-    <t>Feb 2021</t>
-  </si>
-  <si>
-    <t>Jan 2021</t>
-  </si>
-  <si>
-    <t>Dec 2020</t>
-  </si>
-  <si>
-    <t>Nov 2020</t>
-  </si>
-  <si>
-    <t>Oct 2020</t>
-  </si>
-  <si>
-    <t>Sep 2020</t>
-  </si>
-  <si>
-    <t>Aug 2020</t>
-  </si>
-  <si>
-    <t>Jul 2020</t>
-  </si>
-  <si>
-    <t>Jun 2020</t>
-  </si>
-  <si>
-    <t>May 2020</t>
-  </si>
-  <si>
-    <t>Apr 2020</t>
-  </si>
-  <si>
-    <t>Mar 2020</t>
-  </si>
-  <si>
-    <t>Feb 2020</t>
-  </si>
-  <si>
-    <t>Jan 2020</t>
+    <t>TradeType</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="m/d/yyyy;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -602,7 +495,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -923,7 +816,7 @@
   <dimension ref="A1:AL309"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C1" sqref="C1:AL1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -932,7 +825,9 @@
     <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="38" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="38" width="11.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.35">
@@ -940,123 +835,123 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="O1" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="P1" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q1" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="R1" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="S1" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="T1" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="U1" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="V1" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="W1" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="X1" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="Y1" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="Z1" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="AA1" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="AB1" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="AC1" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="AD1" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="AE1" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="AF1" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="AG1" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="AH1" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="AI1" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="AJ1" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="AK1" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="AL1" s="9" t="s">
-        <v>152</v>
+        <v>116</v>
+      </c>
+      <c r="C1" s="9">
+        <v>44896</v>
+      </c>
+      <c r="D1" s="9">
+        <v>44866</v>
+      </c>
+      <c r="E1" s="9">
+        <v>44835</v>
+      </c>
+      <c r="F1" s="9">
+        <v>44805</v>
+      </c>
+      <c r="G1" s="9">
+        <v>44774</v>
+      </c>
+      <c r="H1" s="9">
+        <v>44743</v>
+      </c>
+      <c r="I1" s="9">
+        <v>44713</v>
+      </c>
+      <c r="J1" s="9">
+        <v>44682</v>
+      </c>
+      <c r="K1" s="9">
+        <v>44652</v>
+      </c>
+      <c r="L1" s="9">
+        <v>44621</v>
+      </c>
+      <c r="M1" s="9">
+        <v>44593</v>
+      </c>
+      <c r="N1" s="9">
+        <v>44562</v>
+      </c>
+      <c r="O1" s="9">
+        <v>44531</v>
+      </c>
+      <c r="P1" s="9">
+        <v>44501</v>
+      </c>
+      <c r="Q1" s="9">
+        <v>44470</v>
+      </c>
+      <c r="R1" s="9">
+        <v>44440</v>
+      </c>
+      <c r="S1" s="9">
+        <v>44409</v>
+      </c>
+      <c r="T1" s="9">
+        <v>44378</v>
+      </c>
+      <c r="U1" s="9">
+        <v>44348</v>
+      </c>
+      <c r="V1" s="9">
+        <v>44317</v>
+      </c>
+      <c r="W1" s="9">
+        <v>44287</v>
+      </c>
+      <c r="X1" s="9">
+        <v>44256</v>
+      </c>
+      <c r="Y1" s="9">
+        <v>44228</v>
+      </c>
+      <c r="Z1" s="9">
+        <v>44197</v>
+      </c>
+      <c r="AA1" s="9">
+        <v>44166</v>
+      </c>
+      <c r="AB1" s="9">
+        <v>44136</v>
+      </c>
+      <c r="AC1" s="9">
+        <v>44105</v>
+      </c>
+      <c r="AD1" s="9">
+        <v>44075</v>
+      </c>
+      <c r="AE1" s="9">
+        <v>44044</v>
+      </c>
+      <c r="AF1" s="9">
+        <v>44013</v>
+      </c>
+      <c r="AG1" s="9">
+        <v>43983</v>
+      </c>
+      <c r="AH1" s="9">
+        <v>43952</v>
+      </c>
+      <c r="AI1" s="9">
+        <v>43922</v>
+      </c>
+      <c r="AJ1" s="9">
+        <v>43891</v>
+      </c>
+      <c r="AK1" s="9">
+        <v>43862</v>
+      </c>
+      <c r="AL1" s="9">
+        <v>43831</v>
       </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>3</v>
       </c>
       <c r="C2" s="4">
         <v>103655</v>
@@ -1169,10 +1064,10 @@
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="4">
         <v>67665</v>
@@ -1285,10 +1180,10 @@
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="4">
         <v>1537347</v>
@@ -1401,10 +1296,10 @@
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="4">
         <v>1129542</v>
@@ -1517,10 +1412,10 @@
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="4">
         <v>99085</v>
@@ -1633,10 +1528,10 @@
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" s="4">
         <v>106678</v>
@@ -1749,10 +1644,10 @@
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" s="4">
         <v>702472</v>
@@ -1865,10 +1760,10 @@
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" s="4">
         <v>8156</v>
@@ -1981,10 +1876,10 @@
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" s="4">
         <v>384010</v>
@@ -2097,10 +1992,10 @@
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11" s="4">
         <v>940088</v>
@@ -2213,10 +2108,10 @@
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12" s="4">
         <v>31026</v>
@@ -2329,10 +2224,10 @@
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13" s="4">
         <v>262629</v>
@@ -2445,10 +2340,10 @@
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14" s="4">
         <v>104665</v>
@@ -2561,10 +2456,10 @@
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C15" s="4">
         <v>42399</v>
@@ -2677,10 +2572,10 @@
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C16" s="4">
         <v>162253</v>
@@ -2793,10 +2688,10 @@
     </row>
     <row r="17" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C17" s="4">
         <v>992687</v>
@@ -2909,10 +2804,10 @@
     </row>
     <row r="18" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C18" s="4">
         <v>41040</v>
@@ -3025,10 +2920,10 @@
     </row>
     <row r="19" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19" s="4">
         <v>0</v>
@@ -3141,10 +3036,10 @@
     </row>
     <row r="20" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C20" s="4">
         <v>44406</v>
@@ -3257,10 +3152,10 @@
     </row>
     <row r="21" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C21" s="4">
         <v>61324</v>
@@ -3373,10 +3268,10 @@
     </row>
     <row r="22" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C22" s="4">
         <v>5378</v>
@@ -3489,10 +3384,10 @@
     </row>
     <row r="23" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C23" s="4">
         <v>4288</v>
@@ -3605,10 +3500,10 @@
     </row>
     <row r="24" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C24" s="4">
         <v>13594</v>
@@ -3721,10 +3616,10 @@
     </row>
     <row r="25" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C25" s="4">
         <v>7106</v>
@@ -3837,10 +3732,10 @@
     </row>
     <row r="26" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C26" s="4">
         <v>69549</v>
@@ -3953,10 +3848,10 @@
     </row>
     <row r="27" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C27" s="4">
         <v>9115</v>
@@ -4069,10 +3964,10 @@
     </row>
     <row r="28" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C28" s="4">
         <v>143124</v>
@@ -4185,10 +4080,10 @@
     </row>
     <row r="29" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C29" s="4">
         <v>2074781</v>
@@ -4301,10 +4196,10 @@
     </row>
     <row r="30" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C30" s="4">
         <v>6017970</v>
@@ -4417,10 +4312,10 @@
     </row>
     <row r="31" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C31" s="4">
         <v>592778</v>
@@ -4533,10 +4428,10 @@
     </row>
     <row r="32" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C32" s="4">
         <v>1116398</v>
@@ -4649,10 +4544,10 @@
     </row>
     <row r="33" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C33" s="4">
         <v>7486</v>
@@ -4765,10 +4660,10 @@
     </row>
     <row r="34" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C34" s="4">
         <v>25899</v>
@@ -4881,10 +4776,10 @@
     </row>
     <row r="35" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C35" s="4">
         <v>7281</v>
@@ -4997,10 +4892,10 @@
     </row>
     <row r="36" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C36" s="4">
         <v>567388</v>
@@ -5113,10 +5008,10 @@
     </row>
     <row r="37" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C37" s="4">
         <v>2618288</v>
@@ -5229,10 +5124,10 @@
     </row>
     <row r="38" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C38" s="4">
         <v>240017</v>
@@ -5345,10 +5240,10 @@
     </row>
     <row r="39" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C39" s="4">
         <v>3207322</v>
@@ -5461,10 +5356,10 @@
     </row>
     <row r="40" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C40" s="4">
         <v>5357878</v>
@@ -5577,10 +5472,10 @@
     </row>
     <row r="41" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C41" s="4">
         <v>1376</v>
@@ -5693,10 +5588,10 @@
     </row>
     <row r="42" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C42" s="4">
         <v>7642587</v>
@@ -5809,10 +5704,10 @@
     </row>
     <row r="43" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C43" s="4">
         <v>61</v>
@@ -5925,10 +5820,10 @@
     </row>
     <row r="44" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C44" s="4">
         <v>27270</v>
@@ -6041,10 +5936,10 @@
     </row>
     <row r="45" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C45" s="4">
         <v>834657</v>
@@ -6157,10 +6052,10 @@
     </row>
     <row r="46" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C46" s="4">
         <v>103</v>
@@ -6273,10 +6168,10 @@
     </row>
     <row r="47" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C47" s="4">
         <v>221</v>
@@ -6389,10 +6284,10 @@
     </row>
     <row r="48" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C48" s="4">
         <v>7334</v>
@@ -6505,10 +6400,10 @@
     </row>
     <row r="49" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C49" s="4">
         <v>10737</v>
@@ -6621,10 +6516,10 @@
     </row>
     <row r="50" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C50" s="4">
         <v>44949</v>
@@ -6737,10 +6632,10 @@
     </row>
     <row r="51" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C51" s="4">
         <v>21698</v>
@@ -6853,10 +6748,10 @@
     </row>
     <row r="52" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C52" s="4">
         <v>317</v>
@@ -6969,10 +6864,10 @@
     </row>
     <row r="53" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C53" s="4">
         <v>98717</v>
@@ -7085,10 +6980,10 @@
     </row>
     <row r="54" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C54" s="4">
         <v>8265</v>
@@ -7201,10 +7096,10 @@
     </row>
     <row r="55" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C55" s="4">
         <v>639</v>
@@ -7317,10 +7212,10 @@
     </row>
     <row r="56" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C56" s="4">
         <v>332</v>
@@ -7433,10 +7328,10 @@
     </row>
     <row r="57" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C57" s="4">
         <v>72624</v>
@@ -7549,10 +7444,10 @@
     </row>
     <row r="58" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C58" s="4">
         <v>640131</v>
@@ -7665,10 +7560,10 @@
     </row>
     <row r="59" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C59" s="4">
         <v>801168</v>
@@ -7781,10 +7676,10 @@
     </row>
     <row r="60" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C60" s="4">
         <v>0</v>
@@ -7897,10 +7792,10 @@
     </row>
     <row r="61" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C61" s="4">
         <v>1212293</v>
@@ -8013,10 +7908,10 @@
     </row>
     <row r="62" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C62" s="4">
         <v>629</v>
@@ -8129,10 +8024,10 @@
     </row>
     <row r="63" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C63" s="4">
         <v>0</v>
@@ -8245,10 +8140,10 @@
     </row>
     <row r="64" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C64" s="4">
         <v>211232</v>
@@ -8361,10 +8256,10 @@
     </row>
     <row r="65" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C65" s="4">
         <v>8375</v>
@@ -8477,10 +8372,10 @@
     </row>
     <row r="66" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C66" s="4">
         <v>5314219</v>
@@ -8593,10 +8488,10 @@
     </row>
     <row r="67" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C67" s="4">
         <v>11273</v>
@@ -8709,10 +8604,10 @@
     </row>
     <row r="68" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C68" s="4">
         <v>1004171</v>
@@ -8825,10 +8720,10 @@
     </row>
     <row r="69" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C69" s="4">
         <v>16649</v>
@@ -8941,10 +8836,10 @@
     </row>
     <row r="70" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C70" s="4">
         <v>7915</v>
@@ -9057,10 +8952,10 @@
     </row>
     <row r="71" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C71" s="4">
         <v>4475</v>
@@ -9173,10 +9068,10 @@
     </row>
     <row r="72" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C72" s="4">
         <v>277739</v>
@@ -9289,10 +9184,10 @@
     </row>
     <row r="73" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C73" s="4">
         <v>681</v>
@@ -9405,10 +9300,10 @@
     </row>
     <row r="74" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C74" s="4">
         <v>3464</v>
@@ -9521,10 +9416,10 @@
     </row>
     <row r="75" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C75" s="4">
         <v>635</v>
@@ -9637,10 +9532,10 @@
     </row>
     <row r="76" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C76" s="4">
         <v>89</v>
@@ -9753,10 +9648,10 @@
     </row>
     <row r="77" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C77" s="4">
         <v>1253373</v>
@@ -9869,10 +9764,10 @@
     </row>
     <row r="78" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C78" s="4">
         <v>243</v>
@@ -9985,10 +9880,10 @@
     </row>
     <row r="79" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C79" s="4">
         <v>18</v>
@@ -10101,10 +9996,10 @@
     </row>
     <row r="80" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C80" s="4">
         <v>122266</v>
@@ -10217,10 +10112,10 @@
     </row>
     <row r="81" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C81" s="4">
         <v>23124</v>
@@ -10333,10 +10228,10 @@
     </row>
     <row r="82" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A82" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C82" s="4">
         <v>210</v>
@@ -10449,10 +10344,10 @@
     </row>
     <row r="83" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A83" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C83" s="4">
         <v>35</v>
@@ -10565,10 +10460,10 @@
     </row>
     <row r="84" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A84" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C84" s="4">
         <v>3</v>
@@ -10681,10 +10576,10 @@
     </row>
     <row r="85" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A85" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C85" s="4">
         <v>1577</v>
@@ -10797,10 +10692,10 @@
     </row>
     <row r="86" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C86" s="4">
         <v>50581</v>
@@ -10913,10 +10808,10 @@
     </row>
     <row r="87" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A87" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C87" s="4">
         <v>2250</v>
@@ -11029,10 +10924,10 @@
     </row>
     <row r="88" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A88" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C88" s="4">
         <v>0</v>
@@ -11145,10 +11040,10 @@
     </row>
     <row r="89" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A89" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C89" s="4">
         <v>127</v>
@@ -11261,10 +11156,10 @@
     </row>
     <row r="90" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C90" s="4">
         <v>11</v>
@@ -11377,10 +11272,10 @@
     </row>
     <row r="91" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A91" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C91" s="4">
         <v>0</v>
@@ -11493,10 +11388,10 @@
     </row>
     <row r="92" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A92" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C92" s="4">
         <v>123</v>
@@ -11609,10 +11504,10 @@
     </row>
     <row r="93" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A93" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C93" s="4">
         <v>6</v>
@@ -11725,10 +11620,10 @@
     </row>
     <row r="94" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A94" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C94" s="4">
         <v>570</v>
@@ -11841,10 +11736,10 @@
     </row>
     <row r="95" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A95" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C95" s="4">
         <v>1457</v>
@@ -11957,10 +11852,10 @@
     </row>
     <row r="96" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A96" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C96" s="4">
         <v>93</v>
@@ -12073,10 +11968,10 @@
     </row>
     <row r="97" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A97" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C97" s="4">
         <v>0</v>
@@ -12189,10 +12084,10 @@
     </row>
     <row r="98" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A98" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C98" s="4">
         <v>64</v>
@@ -12305,10 +12200,10 @@
     </row>
     <row r="99" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A99" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C99" s="4">
         <v>0</v>
@@ -12421,10 +12316,10 @@
     </row>
     <row r="100" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A100" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C100" s="4">
         <v>37931</v>
@@ -12537,10 +12432,10 @@
     </row>
     <row r="101" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A101" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C101" s="4">
         <v>14</v>
@@ -12653,10 +12548,10 @@
     </row>
     <row r="102" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A102" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C102" s="4">
         <v>2</v>
@@ -12769,10 +12664,10 @@
     </row>
     <row r="103" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A103" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C103" s="4">
         <v>46</v>
@@ -12885,10 +12780,10 @@
     </row>
     <row r="104" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A104" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C104" s="4">
         <v>1</v>
@@ -13001,10 +12896,10 @@
     </row>
     <row r="105" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A105" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C105" s="4">
         <v>0</v>
@@ -13117,10 +13012,10 @@
     </row>
     <row r="106" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A106" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C106" s="4">
         <v>0</v>
@@ -13233,10 +13128,10 @@
     </row>
     <row r="107" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A107" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C107" s="4">
         <v>80</v>
@@ -13349,10 +13244,10 @@
     </row>
     <row r="108" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A108" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C108" s="4">
         <v>0</v>
@@ -13465,10 +13360,10 @@
     </row>
     <row r="109" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A109" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C109" s="4">
         <v>0</v>
@@ -13581,10 +13476,10 @@
     </row>
     <row r="110" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A110" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C110" s="4">
         <v>29</v>
@@ -13697,10 +13592,10 @@
     </row>
     <row r="111" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A111" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C111" s="4">
         <v>1</v>
@@ -13813,10 +13708,10 @@
     </row>
     <row r="112" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A112" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C112" s="4">
         <v>33107</v>
@@ -13929,10 +13824,10 @@
     </row>
     <row r="113" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A113" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C113" s="4">
         <v>559381</v>
@@ -14045,10 +13940,10 @@
     </row>
     <row r="114" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A114" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C114" s="4">
         <v>432376</v>
@@ -14161,10 +14056,10 @@
     </row>
     <row r="115" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A115" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C115" s="4">
         <v>31084</v>
@@ -14277,10 +14172,10 @@
     </row>
     <row r="116" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A116" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C116" s="4">
         <v>402218</v>
@@ -14393,10 +14288,10 @@
     </row>
     <row r="117" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A117" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C117" s="4">
         <v>809343</v>
@@ -14509,10 +14404,10 @@
     </row>
     <row r="118" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A118" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C118" s="4">
         <v>131220</v>
@@ -14625,10 +14520,10 @@
     </row>
     <row r="119" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A119" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C119" s="4">
         <v>177243</v>
@@ -14741,10 +14636,10 @@
     </row>
     <row r="120" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A120" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C120" s="4">
         <v>128641</v>
@@ -14857,10 +14752,10 @@
     </row>
     <row r="121" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A121" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C121" s="4">
         <v>25910</v>
@@ -14973,10 +14868,10 @@
     </row>
     <row r="122" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A122" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C122" s="4">
         <v>1243341</v>
@@ -15089,10 +14984,10 @@
     </row>
     <row r="123" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A123" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C123" s="4">
         <v>360897</v>
@@ -15205,10 +15100,10 @@
     </row>
     <row r="124" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A124" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C124" s="4">
         <v>123349</v>
@@ -15321,10 +15216,10 @@
     </row>
     <row r="125" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A125" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C125" s="4">
         <v>46151</v>
@@ -15437,10 +15332,10 @@
     </row>
     <row r="126" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A126" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C126" s="4">
         <v>49367</v>
@@ -15553,10 +15448,10 @@
     </row>
     <row r="127" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A127" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C127" s="4">
         <v>71732</v>
@@ -15669,10 +15564,10 @@
     </row>
     <row r="128" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A128" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C128" s="4">
         <v>14099</v>
@@ -15785,10 +15680,10 @@
     </row>
     <row r="129" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A129" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C129" s="4">
         <v>311701</v>
@@ -15901,10 +15796,10 @@
     </row>
     <row r="130" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A130" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C130" s="4">
         <v>243227</v>
@@ -16017,10 +15912,10 @@
     </row>
     <row r="131" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A131" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C131" s="4">
         <v>0</v>
@@ -16133,10 +16028,10 @@
     </row>
     <row r="132" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A132" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C132" s="4">
         <v>47775</v>
@@ -16249,10 +16144,10 @@
     </row>
     <row r="133" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A133" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C133" s="4">
         <v>53076</v>
@@ -16365,10 +16260,10 @@
     </row>
     <row r="134" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A134" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C134" s="4">
         <v>683</v>
@@ -16481,10 +16376,10 @@
     </row>
     <row r="135" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A135" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C135" s="4">
         <v>7434</v>
@@ -16597,10 +16492,10 @@
     </row>
     <row r="136" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A136" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C136" s="4">
         <v>1248</v>
@@ -16713,10 +16608,10 @@
     </row>
     <row r="137" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A137" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C137" s="4">
         <v>4546</v>
@@ -16829,10 +16724,10 @@
     </row>
     <row r="138" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A138" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C138" s="4">
         <v>23443</v>
@@ -16945,10 +16840,10 @@
     </row>
     <row r="139" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A139" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C139" s="4">
         <v>1217</v>
@@ -17061,10 +16956,10 @@
     </row>
     <row r="140" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A140" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C140" s="4">
         <v>75900</v>
@@ -17177,10 +17072,10 @@
     </row>
     <row r="141" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A141" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C141" s="4">
         <v>3740306</v>
@@ -17293,10 +17188,10 @@
     </row>
     <row r="142" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A142" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C142" s="4">
         <v>5154779</v>
@@ -17409,10 +17304,10 @@
     </row>
     <row r="143" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A143" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C143" s="4">
         <v>1116549</v>
@@ -17525,10 +17420,10 @@
     </row>
     <row r="144" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A144" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C144" s="4">
         <v>1790423</v>
@@ -17641,10 +17536,10 @@
     </row>
     <row r="145" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A145" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C145" s="4">
         <v>449544</v>
@@ -17757,10 +17652,10 @@
     </row>
     <row r="146" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A146" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C146" s="4">
         <v>195030</v>
@@ -17873,10 +17768,10 @@
     </row>
     <row r="147" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A147" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C147" s="4">
         <v>4643</v>
@@ -17989,10 +17884,10 @@
     </row>
     <row r="148" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A148" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C148" s="4">
         <v>1958783</v>
@@ -18105,10 +18000,10 @@
     </row>
     <row r="149" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A149" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C149" s="4">
         <v>2271626</v>
@@ -18221,10 +18116,10 @@
     </row>
     <row r="150" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A150" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C150" s="4">
         <v>7403998</v>
@@ -18337,10 +18232,10 @@
     </row>
     <row r="151" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A151" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C151" s="4">
         <v>2865718</v>
@@ -18453,10 +18348,10 @@
     </row>
     <row r="152" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A152" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C152" s="4">
         <v>2768573</v>
@@ -18569,10 +18464,10 @@
     </row>
     <row r="153" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A153" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C153" s="4">
         <v>29319</v>
@@ -18685,10 +18580,10 @@
     </row>
     <row r="154" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A154" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C154" s="4">
         <v>6374198</v>
@@ -18801,10 +18696,10 @@
     </row>
     <row r="155" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A155" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C155" s="4">
         <v>214</v>
@@ -18917,10 +18812,10 @@
     </row>
     <row r="156" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A156" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C156" s="4">
         <v>294037</v>
@@ -19033,10 +18928,10 @@
     </row>
     <row r="157" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A157" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C157" s="4">
         <v>1703023</v>
@@ -19149,10 +19044,10 @@
     </row>
     <row r="158" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A158" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C158" s="4">
         <v>27931</v>
@@ -19265,10 +19160,10 @@
     </row>
     <row r="159" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A159" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C159" s="4">
         <v>18692</v>
@@ -19381,10 +19276,10 @@
     </row>
     <row r="160" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A160" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C160" s="4">
         <v>183923</v>
@@ -19497,10 +19392,10 @@
     </row>
     <row r="161" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A161" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C161" s="4">
         <v>134049</v>
@@ -19613,10 +19508,10 @@
     </row>
     <row r="162" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A162" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C162" s="4">
         <v>24163</v>
@@ -19729,10 +19624,10 @@
     </row>
     <row r="163" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A163" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C163" s="4">
         <v>48818</v>
@@ -19845,10 +19740,10 @@
     </row>
     <row r="164" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A164" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C164" s="4">
         <v>510</v>
@@ -19961,10 +19856,10 @@
     </row>
     <row r="165" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A165" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C165" s="4">
         <v>105746</v>
@@ -20077,10 +19972,10 @@
     </row>
     <row r="166" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A166" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C166" s="4">
         <v>15012</v>
@@ -20193,10 +20088,10 @@
     </row>
     <row r="167" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A167" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C167" s="4">
         <v>46086</v>
@@ -20309,10 +20204,10 @@
     </row>
     <row r="168" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A168" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C168" s="4">
         <v>1729</v>
@@ -20425,10 +20320,10 @@
     </row>
     <row r="169" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A169" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C169" s="4">
         <v>18234</v>
@@ -20541,10 +20436,10 @@
     </row>
     <row r="170" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A170" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C170" s="4">
         <v>64520</v>
@@ -20657,10 +20552,10 @@
     </row>
     <row r="171" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A171" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C171" s="4">
         <v>102899</v>
@@ -20773,10 +20668,10 @@
     </row>
     <row r="172" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A172" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C172" s="4">
         <v>260</v>
@@ -20889,10 +20784,10 @@
     </row>
     <row r="173" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A173" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C173" s="4">
         <v>625765</v>
@@ -21005,10 +20900,10 @@
     </row>
     <row r="174" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A174" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C174" s="4">
         <v>566</v>
@@ -21121,10 +21016,10 @@
     </row>
     <row r="175" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A175" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C175" s="4">
         <v>0</v>
@@ -21237,10 +21132,10 @@
     </row>
     <row r="176" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A176" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C176" s="4">
         <v>113586</v>
@@ -21353,10 +21248,10 @@
     </row>
     <row r="177" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A177" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C177" s="4">
         <v>4234</v>
@@ -21469,10 +21364,10 @@
     </row>
     <row r="178" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A178" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C178" s="4">
         <v>4671228</v>
@@ -21585,10 +21480,10 @@
     </row>
     <row r="179" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A179" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C179" s="4">
         <v>22119</v>
@@ -21701,10 +21596,10 @@
     </row>
     <row r="180" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A180" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C180" s="4">
         <v>227374</v>
@@ -21817,10 +21712,10 @@
     </row>
     <row r="181" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A181" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C181" s="4">
         <v>8570</v>
@@ -21933,10 +21828,10 @@
     </row>
     <row r="182" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A182" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C182" s="4">
         <v>12036</v>
@@ -22049,10 +21944,10 @@
     </row>
     <row r="183" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A183" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C183" s="4">
         <v>7249</v>
@@ -22165,10 +22060,10 @@
     </row>
     <row r="184" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A184" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C184" s="4">
         <v>224874</v>
@@ -22281,10 +22176,10 @@
     </row>
     <row r="185" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A185" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C185" s="4">
         <v>563</v>
@@ -22397,10 +22292,10 @@
     </row>
     <row r="186" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A186" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C186" s="4">
         <v>11791</v>
@@ -22513,10 +22408,10 @@
     </row>
     <row r="187" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A187" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C187" s="4">
         <v>3822</v>
@@ -22629,10 +22524,10 @@
     </row>
     <row r="188" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A188" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C188" s="4">
         <v>39</v>
@@ -22745,10 +22640,10 @@
     </row>
     <row r="189" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A189" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C189" s="4">
         <v>1711317</v>
@@ -22861,10 +22756,10 @@
     </row>
     <row r="190" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A190" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C190" s="4">
         <v>71371</v>
@@ -22977,10 +22872,10 @@
     </row>
     <row r="191" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A191" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C191" s="4">
         <v>32546</v>
@@ -23093,10 +22988,10 @@
     </row>
     <row r="192" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A192" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C192" s="4">
         <v>397788</v>
@@ -23209,10 +23104,10 @@
     </row>
     <row r="193" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A193" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C193" s="4">
         <v>84412</v>
@@ -23325,10 +23220,10 @@
     </row>
     <row r="194" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A194" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C194" s="4">
         <v>2428</v>
@@ -23441,10 +23336,10 @@
     </row>
     <row r="195" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A195" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C195" s="4">
         <v>41150</v>
@@ -23557,10 +23452,10 @@
     </row>
     <row r="196" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A196" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C196" s="4">
         <v>6018</v>
@@ -23673,10 +23568,10 @@
     </row>
     <row r="197" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A197" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C197" s="4">
         <v>691400</v>
@@ -23789,10 +23684,10 @@
     </row>
     <row r="198" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A198" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C198" s="7">
         <v>328721</v>
@@ -23905,10 +23800,10 @@
     </row>
     <row r="199" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A199" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C199" s="7">
         <v>-36581</v>
@@ -24021,10 +23916,10 @@
     </row>
     <row r="200" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A200" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C200" s="7">
         <v>-1135129</v>
@@ -24137,10 +24032,10 @@
     </row>
     <row r="201" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A201" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C201" s="7">
         <v>-320199</v>
@@ -24253,10 +24148,10 @@
     </row>
     <row r="202" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A202" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C202" s="7">
         <v>32135</v>
@@ -24369,10 +24264,10 @@
     </row>
     <row r="203" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A203" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C203" s="7">
         <v>70565</v>
@@ -24485,10 +24380,10 @@
     </row>
     <row r="204" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A204" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C204" s="7">
         <v>-573831</v>
@@ -24601,10 +24496,10 @@
     </row>
     <row r="205" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A205" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C205" s="7">
         <v>17754</v>
@@ -24717,10 +24612,10 @@
     </row>
     <row r="206" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A206" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C206" s="7">
         <v>859331</v>
@@ -24833,10 +24728,10 @@
     </row>
     <row r="207" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A207" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C207" s="7">
         <v>-579191</v>
@@ -24949,10 +24844,10 @@
     </row>
     <row r="208" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A208" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C208" s="7">
         <v>92323</v>
@@ -25065,10 +24960,10 @@
     </row>
     <row r="209" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A209" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C209" s="7">
         <v>-216478</v>
@@ -25181,10 +25076,10 @@
     </row>
     <row r="210" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A210" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C210" s="7">
         <v>-55298</v>
@@ -25297,10 +25192,10 @@
     </row>
     <row r="211" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A211" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C211" s="7">
         <v>29333</v>
@@ -25413,10 +25308,10 @@
     </row>
     <row r="212" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A212" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C212" s="7">
         <v>-148154</v>
@@ -25529,10 +25424,10 @@
     </row>
     <row r="213" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A213" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C213" s="7">
         <v>-680986</v>
@@ -25645,10 +25540,10 @@
     </row>
     <row r="214" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A214" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C214" s="7">
         <v>202187</v>
@@ -25761,10 +25656,10 @@
     </row>
     <row r="215" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A215" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C215" s="7">
         <v>0</v>
@@ -25877,10 +25772,10 @@
     </row>
     <row r="216" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A216" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C216" s="7">
         <v>3369</v>
@@ -25993,10 +25888,10 @@
     </row>
     <row r="217" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A217" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C217" s="7">
         <v>-8248</v>
@@ -26109,10 +26004,10 @@
     </row>
     <row r="218" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A218" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C218" s="7">
         <v>-4695</v>
@@ -26225,10 +26120,10 @@
     </row>
     <row r="219" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A219" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C219" s="7">
         <v>3146</v>
@@ -26341,10 +26236,10 @@
     </row>
     <row r="220" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A220" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C220" s="7">
         <v>-12346</v>
@@ -26457,10 +26352,10 @@
     </row>
     <row r="221" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A221" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C221" s="7">
         <v>-2560</v>
@@ -26573,10 +26468,10 @@
     </row>
     <row r="222" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A222" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C222" s="7">
         <v>-46106</v>
@@ -26689,10 +26584,10 @@
     </row>
     <row r="223" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A223" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C223" s="7">
         <v>-7898</v>
@@ -26805,10 +26700,10 @@
     </row>
     <row r="224" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A224" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C224" s="7">
         <v>-67224</v>
@@ -26921,10 +26816,10 @@
     </row>
     <row r="225" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A225" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C225" s="7">
         <v>1665525</v>
@@ -27037,10 +26932,10 @@
     </row>
     <row r="226" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A226" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B226" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C226" s="7">
         <v>-863191</v>
@@ -27153,10 +27048,10 @@
     </row>
     <row r="227" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A227" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B227" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C227" s="7">
         <v>523771</v>
@@ -27269,10 +27164,10 @@
     </row>
     <row r="228" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A228" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B228" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C228" s="7">
         <v>674025</v>
@@ -27385,10 +27280,10 @@
     </row>
     <row r="229" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A229" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C229" s="7">
         <v>442058</v>
@@ -27501,10 +27396,10 @@
     </row>
     <row r="230" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A230" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C230" s="7">
         <v>169131</v>
@@ -27617,10 +27512,10 @@
     </row>
     <row r="231" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A231" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C231" s="7">
         <v>-2638</v>
@@ -27733,10 +27628,10 @@
     </row>
     <row r="232" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A232" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C232" s="7">
         <v>1391395</v>
@@ -27849,10 +27744,10 @@
     </row>
     <row r="233" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A233" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C233" s="7">
         <v>-346662</v>
@@ -27965,10 +27860,10 @@
     </row>
     <row r="234" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A234" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C234" s="7">
         <v>7163981</v>
@@ -28081,10 +27976,10 @@
     </row>
     <row r="235" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A235" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C235" s="7">
         <v>-341604</v>
@@ -28197,10 +28092,10 @@
     </row>
     <row r="236" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A236" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C236" s="7">
         <v>-2589305</v>
@@ -28313,10 +28208,10 @@
     </row>
     <row r="237" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A237" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C237" s="7">
         <v>27943</v>
@@ -28429,10 +28324,10 @@
     </row>
     <row r="238" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A238" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C238" s="7">
         <v>-1268389</v>
@@ -28545,10 +28440,10 @@
     </row>
     <row r="239" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A239" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C239" s="7">
         <v>153</v>
@@ -28661,10 +28556,10 @@
     </row>
     <row r="240" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A240" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C240" s="7">
         <v>266767</v>
@@ -28777,10 +28672,10 @@
     </row>
     <row r="241" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A241" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C241" s="7">
         <v>868366</v>
@@ -28893,10 +28788,10 @@
     </row>
     <row r="242" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A242" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C242" s="7">
         <v>27828</v>
@@ -29009,10 +28904,10 @@
     </row>
     <row r="243" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A243" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C243" s="7">
         <v>18471</v>
@@ -29125,10 +29020,10 @@
     </row>
     <row r="244" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A244" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C244" s="7">
         <v>176589</v>
@@ -29241,10 +29136,10 @@
     </row>
     <row r="245" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A245" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C245" s="7">
         <v>123312</v>
@@ -29357,10 +29252,10 @@
     </row>
     <row r="246" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A246" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C246" s="7">
         <v>-20786</v>
@@ -29473,10 +29368,10 @@
     </row>
     <row r="247" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A247" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C247" s="7">
         <v>27120</v>
@@ -29589,10 +29484,10 @@
     </row>
     <row r="248" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A248" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C248" s="7">
         <v>193</v>
@@ -29705,10 +29600,10 @@
     </row>
     <row r="249" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A249" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C249" s="7">
         <v>7029</v>
@@ -29821,10 +29716,10 @@
     </row>
     <row r="250" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A250" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C250" s="7">
         <v>6747</v>
@@ -29937,10 +29832,10 @@
     </row>
     <row r="251" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A251" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C251" s="7">
         <v>45447</v>
@@ -30053,10 +29948,10 @@
     </row>
     <row r="252" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A252" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C252" s="7">
         <v>1397</v>
@@ -30169,10 +30064,10 @@
     </row>
     <row r="253" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A253" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C253" s="7">
         <v>-54390</v>
@@ -30285,10 +30180,10 @@
     </row>
     <row r="254" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A254" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C254" s="7">
         <v>-575611</v>
@@ -30401,10 +30296,10 @@
     </row>
     <row r="255" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A255" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C255" s="7">
         <v>-698269</v>
@@ -30517,10 +30412,10 @@
     </row>
     <row r="256" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A256" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C256" s="7">
         <v>260</v>
@@ -30633,10 +30528,10 @@
     </row>
     <row r="257" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A257" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C257" s="7">
         <v>-586528</v>
@@ -30749,10 +30644,10 @@
     </row>
     <row r="258" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A258" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C258" s="7">
         <v>-63</v>
@@ -30865,10 +30760,10 @@
     </row>
     <row r="259" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A259" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C259" s="7">
         <v>0</v>
@@ -30981,10 +30876,10 @@
     </row>
     <row r="260" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A260" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C260" s="7">
         <v>-97646</v>
@@ -31097,10 +30992,10 @@
     </row>
     <row r="261" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A261" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C261" s="7">
         <v>-4141</v>
@@ -31213,10 +31108,10 @@
     </row>
     <row r="262" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A262" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C262" s="7">
         <v>-642991</v>
@@ -31329,10 +31224,10 @@
     </row>
     <row r="263" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A263" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C263" s="7">
         <v>10846</v>
@@ -31445,10 +31340,10 @@
     </row>
     <row r="264" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A264" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C264" s="7">
         <v>-776797</v>
@@ -31561,10 +31456,10 @@
     </row>
     <row r="265" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A265" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C265" s="7">
         <v>-8079</v>
@@ -31677,10 +31572,10 @@
     </row>
     <row r="266" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A266" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C266" s="7">
         <v>4121</v>
@@ -31793,10 +31688,10 @@
     </row>
     <row r="267" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A267" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C267" s="7">
         <v>2774</v>
@@ -31909,10 +31804,10 @@
     </row>
     <row r="268" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A268" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C268" s="7">
         <v>-52865</v>
@@ -32025,10 +31920,10 @@
     </row>
     <row r="269" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A269" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C269" s="7">
         <v>-118</v>
@@ -32141,10 +32036,10 @@
     </row>
     <row r="270" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A270" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C270" s="7">
         <v>8327</v>
@@ -32257,10 +32152,10 @@
     </row>
     <row r="271" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A271" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C271" s="7">
         <v>3187</v>
@@ -32373,10 +32268,10 @@
     </row>
     <row r="272" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A272" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C272" s="7">
         <v>-50</v>
@@ -32489,10 +32384,10 @@
     </row>
     <row r="273" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A273" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C273" s="7">
         <v>457944</v>
@@ -32605,10 +32500,10 @@
     </row>
     <row r="274" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A274" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C274" s="7">
         <v>71128</v>
@@ -32721,10 +32616,10 @@
     </row>
     <row r="275" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A275" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C275" s="7">
         <v>32528</v>
@@ -32837,10 +32732,10 @@
     </row>
     <row r="276" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A276" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C276" s="7">
         <v>275522</v>
@@ -32953,10 +32848,10 @@
     </row>
     <row r="277" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A277" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C277" s="7">
         <v>61288</v>
@@ -33069,10 +32964,10 @@
     </row>
     <row r="278" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A278" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C278" s="7">
         <v>2218</v>
@@ -33185,10 +33080,10 @@
     </row>
     <row r="279" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A279" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C279" s="7">
         <v>41115</v>
@@ -33301,10 +33196,10 @@
     </row>
     <row r="280" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A280" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C280" s="7">
         <v>6015</v>
@@ -33417,10 +33312,10 @@
     </row>
     <row r="281" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A281" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C281" s="7">
         <v>689823</v>
@@ -33533,10 +33428,10 @@
     </row>
     <row r="282" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A282" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C282" s="7">
         <v>-50581</v>
@@ -33649,10 +33544,10 @@
     </row>
     <row r="283" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A283" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C283" s="7">
         <v>-2250</v>
@@ -33765,10 +33660,10 @@
     </row>
     <row r="284" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A284" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C284" s="7">
         <v>0</v>
@@ -33881,10 +33776,10 @@
     </row>
     <row r="285" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A285" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C285" s="7">
         <v>-127</v>
@@ -33997,10 +33892,10 @@
     </row>
     <row r="286" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A286" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C286" s="7">
         <v>-11</v>
@@ -34113,10 +34008,10 @@
     </row>
     <row r="287" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A287" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C287" s="7">
         <v>0</v>
@@ -34229,10 +34124,10 @@
     </row>
     <row r="288" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A288" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C288" s="7">
         <v>-123</v>
@@ -34345,10 +34240,10 @@
     </row>
     <row r="289" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A289" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C289" s="7">
         <v>-6</v>
@@ -34461,10 +34356,10 @@
     </row>
     <row r="290" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A290" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C290" s="7">
         <v>-570</v>
@@ -34577,10 +34472,10 @@
     </row>
     <row r="291" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A291" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C291" s="7">
         <v>-1457</v>
@@ -34693,10 +34588,10 @@
     </row>
     <row r="292" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A292" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C292" s="7">
         <v>-93</v>
@@ -34809,10 +34704,10 @@
     </row>
     <row r="293" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A293" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C293" s="7">
         <v>0</v>
@@ -34925,10 +34820,10 @@
     </row>
     <row r="294" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A294" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C294" s="7">
         <v>-64</v>
@@ -35041,10 +34936,10 @@
     </row>
     <row r="295" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A295" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C295" s="7">
         <v>0</v>
@@ -35157,10 +35052,10 @@
     </row>
     <row r="296" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A296" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C296" s="7">
         <v>-37931</v>
@@ -35273,10 +35168,10 @@
     </row>
     <row r="297" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A297" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C297" s="7">
         <v>-14</v>
@@ -35389,10 +35284,10 @@
     </row>
     <row r="298" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A298" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C298" s="7">
         <v>-2</v>
@@ -35505,10 +35400,10 @@
     </row>
     <row r="299" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A299" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C299" s="7">
         <v>-46</v>
@@ -35621,10 +35516,10 @@
     </row>
     <row r="300" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A300" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C300" s="7">
         <v>-1</v>
@@ -35737,10 +35632,10 @@
     </row>
     <row r="301" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A301" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C301" s="7">
         <v>0</v>
@@ -35853,10 +35748,10 @@
     </row>
     <row r="302" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A302" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C302" s="7">
         <v>0</v>
@@ -35969,10 +35864,10 @@
     </row>
     <row r="303" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A303" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C303" s="7">
         <v>-80</v>
@@ -36085,10 +35980,10 @@
     </row>
     <row r="304" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A304" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C304" s="7">
         <v>0</v>
@@ -36201,10 +36096,10 @@
     </row>
     <row r="305" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A305" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B305" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C305" s="7">
         <v>0</v>
@@ -36317,10 +36212,10 @@
     </row>
     <row r="306" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A306" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B306" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C306" s="7">
         <v>-29</v>
@@ -36433,10 +36328,10 @@
     </row>
     <row r="307" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A307" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C307" s="7">
         <v>-1</v>
@@ -36549,10 +36444,10 @@
     </row>
     <row r="308" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A308" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C308" s="7">
         <v>-33107</v>
@@ -36665,10 +36560,10 @@
     </row>
     <row r="309" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A309" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B309" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C309" s="7">
         <v>-559381</v>

</xml_diff>